<commit_message>
Add lockdown dates csv
</commit_message>
<xml_diff>
--- a/lockdown_dates.xlsx
+++ b/lockdown_dates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8c0002738dae3070/Bureaublad/Study/Master/BigData/MBD_11/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{383A39D7-A56A-45AD-963B-7F809FCFE300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{383A39D7-A56A-45AD-963B-7F809FCFE300}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C25AF7F7-CD99-43E5-8277-2E864EC33093}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DAC2AC1D-759C-46A8-B898-5D63DDBC456E}"/>
   </bookViews>
@@ -499,10 +499,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C25ADE21-55E4-4B51-B8B9-D3BE09F8B6B4}">
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -515,106 +515,100 @@
     <col min="11" max="11" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="1"/>
-    </row>
-    <row r="2" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="A2" s="1"/>
-      <c r="B2" s="4" t="s">
+    <row r="1" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="B1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="7" t="s">
+    <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="9">
+      <c r="B2" s="9">
         <v>43905</v>
       </c>
-      <c r="D3" s="5">
+      <c r="C2" s="5">
         <v>43962</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
-      <c r="B4" s="8" t="s">
+    <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="10">
+      <c r="B3" s="10">
         <v>44117</v>
       </c>
-      <c r="D4" s="3">
+      <c r="C3" s="3">
         <v>44154</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A5" s="1"/>
-      <c r="B5" s="7" t="s">
+    <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="9">
+      <c r="B4" s="9">
         <v>44180</v>
       </c>
-      <c r="D5" s="5">
+      <c r="C4" s="5">
         <v>44314</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
-      <c r="A6" s="1"/>
-      <c r="B6" s="8" t="s">
+    <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="10">
+      <c r="B5" s="10">
         <v>44314</v>
       </c>
-      <c r="D6" s="3">
+      <c r="C5" s="3">
         <v>44373</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="17.25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="9">
+        <v>44544</v>
+      </c>
+      <c r="C6" s="5">
+        <v>44587</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>
-      <c r="B7" s="7" t="s">
-        <v>4</v>
-      </c>
-      <c r="C7" s="9">
-        <v>44544</v>
-      </c>
-      <c r="D7" s="5">
-        <v>44587</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
     </row>
-    <row r="9" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
-    <row r="10" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
     </row>
-    <row r="11" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A11" s="2"/>
     </row>
-    <row r="12" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
     </row>
-    <row r="13" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
     </row>
-    <row r="14" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
     </row>
-    <row r="15" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
     </row>
-    <row r="16" spans="1:4" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
     </row>
     <row r="17" spans="1:1" ht="17.25" x14ac:dyDescent="0.25">

</xml_diff>